<commit_message>
* v1.0.19 Updating for different macOS devices. Addressing reviewer comments.
</commit_message>
<xml_diff>
--- a/MCP1_pg_mL/BASELINE/20200714.MCP1_pg_mL.AE.BaselineTable.subsetCEA.xlsx
+++ b/MCP1_pg_mL/BASELINE/20200714.MCP1_pg_mL.AE.BaselineTable.subsetCEA.xlsx
@@ -89,7 +89,7 @@
     <t xml:space="preserve">    0.0 (   0) </t>
   </si>
   <si>
-    <t xml:space="preserve"> NaN</t>
+    <t xml:space="preserve">   NaN</t>
   </si>
   <si>
     <t xml:space="preserve">X.1</t>
@@ -2090,7 +2090,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">

</xml_diff>